<commit_message>
#3518 - Update Personnel and Investment Item Template
</commit_message>
<xml_diff>
--- a/pabi_budget_plan/xlsx_template/Budget_Plan_HREXP_Budget_20180803-form.xlsx
+++ b/pabi_budget_plan/xlsx_template/Budget_Plan_HREXP_Budget_20180803-form.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t xml:space="preserve">Fiscal Year</t>
   </si>
@@ -115,9 +115,6 @@
     <t xml:space="preserve">External</t>
   </si>
   <si>
-    <t xml:space="preserve">109999</t>
-  </si>
-  <si>
     <t xml:space="preserve">เงินเดือนและสวัสดิการ</t>
   </si>
   <si>
@@ -125,18 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve">สวัสดิการ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">209999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">309999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">409999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">509999</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL </t>
@@ -256,16 +241,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="222"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="222"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="222"/>
     </font>
     <font>
       <sz val="10"/>
@@ -913,21 +901,21 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="0.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="36.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="30.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="8" style="1" width="25.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="23" style="1" width="8.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="1" width="8.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="0.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="36.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="8" style="1" width="25.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="23" style="1" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="1" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="5.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -994,7 +982,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="4.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="4.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="8" t="s">
         <v>6</v>
@@ -1074,7 +1062,7 @@
       </c>
       <c r="W8" s="18"/>
     </row>
-    <row r="9" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="19" t="s">
         <v>28</v>
       </c>
@@ -1082,18 +1070,18 @@
         <f aca="false">IF($D9="","",VLOOKUP(LEFT($D9,1),TAB_List!$B$5:$F$12,2,0))</f>
         <v>สก.</v>
       </c>
-      <c r="D9" s="20" t="s">
-        <v>29</v>
+      <c r="D9" s="20" t="n">
+        <v>1099999</v>
       </c>
       <c r="E9" s="20" t="str">
         <f aca="false">IF($D9="","","งบบุคลากรเงินเดือนและสวัสดิการ "&amp;$C9)</f>
         <v>งบบุคลากรเงินเดือนและสวัสดิการ สก.</v>
       </c>
       <c r="F9" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="21" t="s">
         <v>30</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>31</v>
       </c>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
@@ -1121,7 +1109,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="19" t="s">
         <v>28</v>
       </c>
@@ -1129,18 +1117,18 @@
         <f aca="false">IF($D10="","",VLOOKUP(LEFT($D10,1),TAB_List!$B$5:$F$12,2,0))</f>
         <v>สก.</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>29</v>
+      <c r="D10" s="20" t="n">
+        <v>1099999</v>
       </c>
       <c r="E10" s="20" t="str">
         <f aca="false">IF($D10="","","งบบุคลากรเงินเดือนและสวัสดิการ "&amp;$C10)</f>
         <v>งบบุคลากรเงินเดือนและสวัสดิการ สก.</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
@@ -1168,7 +1156,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="19" t="s">
         <v>28</v>
       </c>
@@ -1177,17 +1165,17 @@
         <v>ศช.</v>
       </c>
       <c r="D11" s="20" t="n">
-        <v>209999</v>
+        <v>2099999</v>
       </c>
       <c r="E11" s="20" t="str">
         <f aca="false">IF($D11="","","งบบุคลากรเงินเดือนและสวัสดิการ "&amp;$C11)</f>
         <v>งบบุคลากรเงินเดือนและสวัสดิการ ศช.</v>
       </c>
       <c r="F11" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="21" t="s">
         <v>30</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>31</v>
       </c>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
@@ -1215,7 +1203,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="19" t="s">
         <v>28</v>
       </c>
@@ -1223,18 +1211,18 @@
         <f aca="false">IF($D12="","",VLOOKUP(LEFT($D12,1),TAB_List!$B$5:$F$12,2,0))</f>
         <v>ศช.</v>
       </c>
-      <c r="D12" s="20" t="s">
-        <v>33</v>
+      <c r="D12" s="20" t="n">
+        <v>2099999</v>
       </c>
       <c r="E12" s="20" t="str">
         <f aca="false">IF($D12="","","งบบุคลากรเงินเดือนและสวัสดิการ "&amp;$C12)</f>
         <v>งบบุคลากรเงินเดือนและสวัสดิการ ศช.</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
@@ -1262,7 +1250,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="19" t="s">
         <v>28</v>
       </c>
@@ -1270,18 +1258,18 @@
         <f aca="false">IF($D13="","",VLOOKUP(LEFT($D13,1),TAB_List!$B$5:$F$12,2,0))</f>
         <v>ศว.</v>
       </c>
-      <c r="D13" s="20" t="s">
-        <v>34</v>
+      <c r="D13" s="20" t="n">
+        <v>3099999</v>
       </c>
       <c r="E13" s="20" t="str">
         <f aca="false">IF($D13="","","งบบุคลากรเงินเดือนและสวัสดิการ "&amp;$C13)</f>
         <v>งบบุคลากรเงินเดือนและสวัสดิการ ศว.</v>
       </c>
       <c r="F13" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="21" t="s">
         <v>30</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>31</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
@@ -1309,7 +1297,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="19" t="s">
         <v>28</v>
       </c>
@@ -1317,18 +1305,18 @@
         <f aca="false">IF($D14="","",VLOOKUP(LEFT($D14,1),TAB_List!$B$5:$F$12,2,0))</f>
         <v>ศว.</v>
       </c>
-      <c r="D14" s="20" t="s">
-        <v>34</v>
+      <c r="D14" s="20" t="n">
+        <v>3099999</v>
       </c>
       <c r="E14" s="20" t="str">
         <f aca="false">IF($D14="","","งบบุคลากรเงินเดือนและสวัสดิการ "&amp;$C14)</f>
         <v>งบบุคลากรเงินเดือนและสวัสดิการ ศว.</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="22"/>
@@ -1356,7 +1344,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="19" t="s">
         <v>28</v>
       </c>
@@ -1364,18 +1352,18 @@
         <f aca="false">IF($D15="","",VLOOKUP(LEFT($D15,1),TAB_List!$B$5:$F$12,2,0))</f>
         <v>ศอ.</v>
       </c>
-      <c r="D15" s="20" t="s">
-        <v>35</v>
+      <c r="D15" s="20" t="n">
+        <v>4099999</v>
       </c>
       <c r="E15" s="20" t="str">
         <f aca="false">IF($D15="","","งบบุคลากรเงินเดือนและสวัสดิการ "&amp;$C15)</f>
         <v>งบบุคลากรเงินเดือนและสวัสดิการ ศอ.</v>
       </c>
       <c r="F15" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="21" t="s">
         <v>30</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>31</v>
       </c>
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
@@ -1403,7 +1391,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="19" t="s">
         <v>28</v>
       </c>
@@ -1411,18 +1399,18 @@
         <f aca="false">IF($D16="","",VLOOKUP(LEFT($D16,1),TAB_List!$B$5:$F$12,2,0))</f>
         <v>ศอ.</v>
       </c>
-      <c r="D16" s="20" t="s">
-        <v>35</v>
+      <c r="D16" s="20" t="n">
+        <v>4099999</v>
       </c>
       <c r="E16" s="20" t="str">
         <f aca="false">IF($D16="","","งบบุคลากรเงินเดือนและสวัสดิการ "&amp;$C16)</f>
         <v>งบบุคลากรเงินเดือนและสวัสดิการ ศอ.</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
@@ -1450,7 +1438,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="19" t="s">
         <v>28</v>
       </c>
@@ -1458,18 +1446,18 @@
         <f aca="false">IF($D17="","",VLOOKUP(LEFT($D17,1),TAB_List!$B$5:$F$12,2,0))</f>
         <v>ศน.</v>
       </c>
-      <c r="D17" s="20" t="s">
-        <v>36</v>
+      <c r="D17" s="20" t="n">
+        <v>5099999</v>
       </c>
       <c r="E17" s="20" t="str">
         <f aca="false">IF($D17="","","งบบุคลากรเงินเดือนและสวัสดิการ "&amp;$C17)</f>
         <v>งบบุคลากรเงินเดือนและสวัสดิการ ศน.</v>
       </c>
       <c r="F17" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="21" t="s">
         <v>30</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>31</v>
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
@@ -1497,7 +1485,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="19" t="s">
         <v>28</v>
       </c>
@@ -1505,18 +1493,18 @@
         <f aca="false">IF($D18="","",VLOOKUP(LEFT($D18,1),TAB_List!$B$5:$F$12,2,0))</f>
         <v>ศน.</v>
       </c>
-      <c r="D18" s="20" t="s">
-        <v>36</v>
+      <c r="D18" s="20" t="n">
+        <v>5099999</v>
       </c>
       <c r="E18" s="20" t="str">
         <f aca="false">IF($D18="","","งบบุคลากรเงินเดือนและสวัสดิการ "&amp;$C18)</f>
         <v>งบบุคลากรเงินเดือนและสวัสดิการ ศน.</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>
@@ -1856,9 +1844,9 @@
         <v/>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="30" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
@@ -1931,7 +1919,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" password="cf2a" objects="true" scenarios="true"/>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <conditionalFormatting sqref="V9:V12 V19:V26">
     <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NA()</formula>
@@ -2009,124 +1997,124 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="0.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="50.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="8.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="0.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="50.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="8.86"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="4.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1" customFormat="false" ht="4.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="4.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="37"/>
+    </row>
+    <row r="4" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="38" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="4.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="37"/>
-    </row>
-    <row r="4" customFormat="false" ht="25.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="38" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="39" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E5" s="39" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="39" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="39" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="39" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="39" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F9" s="40" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>